<commit_message>
First draft of the scatter plots and heat map
</commit_message>
<xml_diff>
--- a/resources/lat_long.xlsx
+++ b/resources/lat_long.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b77077/Workspace/Analytics/BC_Project/project_1/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361B887D-63B1-C349-A8E8-1BDAC33BA16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A994686-8585-A546-BC5A-6CFB1075EDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5100" yWindow="3700" windowWidth="26840" windowHeight="15940" xr2:uid="{D6615E25-8357-114C-B65F-54244E31E870}"/>
   </bookViews>
@@ -572,6 +572,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>